<commit_message>
cập nhật thống kê và trackingsheet
</commit_message>
<xml_diff>
--- a/Deliverables/Documents/D4H_Trackingsheet_v.1.0.xlsx
+++ b/Deliverables/Documents/D4H_Trackingsheet_v.1.0.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Doc" sheetId="1" r:id="rId1"/>
     <sheet name="Product" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="97">
   <si>
     <t>Doc Name</t>
   </si>
@@ -292,6 +292,21 @@
   </si>
   <si>
     <t>Start date</t>
+  </si>
+  <si>
+    <t>Xác thực tài khoản</t>
+  </si>
+  <si>
+    <t>Tạo chức năng nhập</t>
+  </si>
+  <si>
+    <t>Tạo chức năng xuất</t>
+  </si>
+  <si>
+    <t>Tạo chức năng đăng ký</t>
+  </si>
+  <si>
+    <t>Hoa, Hương</t>
   </si>
 </sst>
 </file>
@@ -479,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -542,12 +557,36 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -602,14 +641,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -914,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,10 +963,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="34"/>
       <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
@@ -941,10 +974,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="4"/>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="28"/>
+      <c r="G1" s="36"/>
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
@@ -961,10 +994,10 @@
       <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
+      <c r="B2" s="35"/>
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
@@ -972,10 +1005,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="28"/>
+      <c r="G2" s="36"/>
       <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1027,10 +1060,10 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="24">
+      <c r="A5" s="29">
         <v>1</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="29" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -1042,26 +1075,26 @@
       <c r="E5" s="10">
         <v>43689</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="30">
         <v>43703</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="30">
         <v>43703</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="30">
         <v>43697</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I5" s="29">
         <v>100</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="J5" s="29" t="s">
         <v>22</v>
       </c>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="9" t="s">
         <v>21</v>
       </c>
@@ -1071,18 +1104,18 @@
       <c r="E6" s="10">
         <v>43702</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
       <c r="K6" s="8"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="24">
+      <c r="A7" s="29">
         <v>2</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="29" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -1112,8 +1145,8 @@
       <c r="K7" s="8"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="8" t="s">
         <v>27</v>
       </c>
@@ -1141,10 +1174,10 @@
       <c r="K8" s="8"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="24">
+      <c r="A9" s="29">
         <v>3</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="29" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -1153,10 +1186,10 @@
       <c r="D9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="44">
+      <c r="E9" s="31">
         <v>43720</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="30">
         <v>43728</v>
       </c>
       <c r="G9" s="10">
@@ -1165,61 +1198,61 @@
       <c r="H9" s="10">
         <v>43728</v>
       </c>
-      <c r="I9" s="24">
+      <c r="I9" s="29">
         <v>100</v>
       </c>
-      <c r="J9" s="24" t="s">
+      <c r="J9" s="29" t="s">
         <v>22</v>
       </c>
       <c r="K9" s="8"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="8" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="45"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="30"/>
       <c r="G10" s="10">
         <v>43728</v>
       </c>
       <c r="H10" s="10">
         <v>43728</v>
       </c>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
       <c r="K10" s="8"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="46"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="30"/>
       <c r="G11" s="10">
         <v>43728</v>
       </c>
       <c r="H11" s="10">
         <v>43728</v>
       </c>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
       <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="24">
+      <c r="A12" s="29">
         <v>4</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -1228,10 +1261,10 @@
       <c r="D12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="44">
+      <c r="E12" s="31">
         <v>43708</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="30">
         <v>43734</v>
       </c>
       <c r="G12" s="10">
@@ -1240,126 +1273,126 @@
       <c r="H12" s="10">
         <v>43708</v>
       </c>
-      <c r="I12" s="24">
+      <c r="I12" s="29">
         <v>100</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="J12" s="29" t="s">
         <v>22</v>
       </c>
       <c r="K12" s="8"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="8" t="s">
         <v>36</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="45"/>
-      <c r="F13" s="25"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="30"/>
       <c r="G13" s="10">
         <v>43710</v>
       </c>
       <c r="H13" s="10">
         <v>43710</v>
       </c>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
       <c r="K13" s="8"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="8" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="45"/>
-      <c r="F14" s="25"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="30"/>
       <c r="G14" s="10">
         <v>43710</v>
       </c>
       <c r="H14" s="10">
         <v>43710</v>
       </c>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
       <c r="K14" s="8"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="45"/>
-      <c r="F15" s="25"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="30"/>
       <c r="G15" s="10">
         <v>43710</v>
       </c>
       <c r="H15" s="10">
         <v>43710</v>
       </c>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
       <c r="K15" s="8"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="8" t="s">
         <v>39</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="45"/>
-      <c r="F16" s="25"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="30"/>
       <c r="G16" s="10">
         <v>43710</v>
       </c>
       <c r="H16" s="10">
         <v>43712</v>
       </c>
-      <c r="I16" s="24"/>
+      <c r="I16" s="29"/>
       <c r="J16" s="8" t="s">
         <v>71</v>
       </c>
       <c r="K16" s="8"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="46"/>
-      <c r="F17" s="25"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="30"/>
       <c r="G17" s="10">
         <v>43710</v>
       </c>
       <c r="H17" s="10">
         <v>43710</v>
       </c>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24" t="s">
+      <c r="I17" s="29"/>
+      <c r="J17" s="29" t="s">
         <v>22</v>
       </c>
       <c r="K17" s="8"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="B18" s="24"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="8" t="s">
         <v>45</v>
       </c>
@@ -1369,20 +1402,20 @@
       <c r="E18" s="10">
         <v>43713</v>
       </c>
-      <c r="F18" s="25"/>
+      <c r="F18" s="30"/>
       <c r="G18" s="10">
         <v>43713</v>
       </c>
       <c r="H18" s="10">
         <v>43713</v>
       </c>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
       <c r="K18" s="8"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="8" t="s">
         <v>47</v>
       </c>
@@ -1392,22 +1425,22 @@
       <c r="E19" s="10">
         <v>43716</v>
       </c>
-      <c r="F19" s="25"/>
+      <c r="F19" s="30"/>
       <c r="G19" s="10">
         <v>43716</v>
       </c>
       <c r="H19" s="10">
         <v>43716</v>
       </c>
-      <c r="I19" s="24"/>
+      <c r="I19" s="29"/>
       <c r="J19" s="8" t="s">
         <v>72</v>
       </c>
       <c r="K19" s="8"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="24"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="8" t="s">
         <v>68</v>
       </c>
@@ -1417,22 +1450,22 @@
       <c r="E20" s="10">
         <v>43720</v>
       </c>
-      <c r="F20" s="25"/>
+      <c r="F20" s="30"/>
       <c r="G20" s="10">
         <v>43723</v>
       </c>
       <c r="H20" s="10">
         <v>43723</v>
       </c>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24" t="s">
+      <c r="I20" s="29"/>
+      <c r="J20" s="29" t="s">
         <v>22</v>
       </c>
       <c r="K20" s="8"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
-      <c r="B21" s="24"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="8" t="s">
         <v>49</v>
       </c>
@@ -1442,22 +1475,22 @@
       <c r="E21" s="10">
         <v>43725</v>
       </c>
-      <c r="F21" s="25"/>
+      <c r="F21" s="30"/>
       <c r="G21" s="10">
         <v>43725</v>
       </c>
       <c r="H21" s="10">
         <v>43725</v>
       </c>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
       <c r="K21" s="8"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="24">
+      <c r="A22" s="29">
         <v>5</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="29" t="s">
         <v>50</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -1466,10 +1499,10 @@
       <c r="D22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="44">
+      <c r="E22" s="31">
         <v>43726</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="30">
         <v>43728</v>
       </c>
       <c r="G22" s="10">
@@ -1478,143 +1511,143 @@
       <c r="H22" s="10">
         <v>43726</v>
       </c>
-      <c r="I22" s="24">
+      <c r="I22" s="29">
         <v>100</v>
       </c>
-      <c r="J22" s="24" t="s">
+      <c r="J22" s="29" t="s">
         <v>22</v>
       </c>
       <c r="K22" s="8"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
-      <c r="B23" s="24"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="8" t="s">
         <v>52</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="45"/>
-      <c r="F23" s="25"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="30"/>
       <c r="G23" s="10">
         <v>43727</v>
       </c>
       <c r="H23" s="10">
         <v>43727</v>
       </c>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
       <c r="K23" s="8"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
       <c r="C24" s="8" t="s">
         <v>53</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="45"/>
-      <c r="F24" s="25"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="30"/>
       <c r="G24" s="10">
         <v>43727</v>
       </c>
       <c r="H24" s="10">
         <v>43727</v>
       </c>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
       <c r="K24" s="8"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="8" t="s">
         <v>54</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="45"/>
-      <c r="F25" s="25"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="30"/>
       <c r="G25" s="10">
         <v>43727</v>
       </c>
       <c r="H25" s="10">
         <v>43727</v>
       </c>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
       <c r="K25" s="8"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
-      <c r="B26" s="24"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
       <c r="C26" s="8" t="s">
         <v>55</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="45"/>
-      <c r="F26" s="25"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="30"/>
       <c r="G26" s="10">
         <v>43727</v>
       </c>
       <c r="H26" s="10">
         <v>43727</v>
       </c>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
       <c r="K26" s="8"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
-      <c r="B27" s="24"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="8" t="s">
         <v>56</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E27" s="45"/>
-      <c r="F27" s="25"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="30"/>
       <c r="G27" s="10">
         <v>43727</v>
       </c>
       <c r="H27" s="10">
         <v>43727</v>
       </c>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
       <c r="K27" s="8"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
-      <c r="B28" s="24"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="8" t="s">
         <v>57</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="46"/>
-      <c r="F28" s="25"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="30"/>
       <c r="G28" s="10">
         <v>43727</v>
       </c>
       <c r="H28" s="10">
         <v>43727</v>
       </c>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
       <c r="K28" s="8"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
-      <c r="B29" s="24"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
       <c r="C29" s="8" t="s">
         <v>58</v>
       </c>
@@ -1624,20 +1657,20 @@
       <c r="E29" s="10">
         <v>43727</v>
       </c>
-      <c r="F29" s="25"/>
+      <c r="F29" s="30"/>
       <c r="G29" s="10">
         <v>43727</v>
       </c>
       <c r="H29" s="10">
         <v>43727</v>
       </c>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
       <c r="K29" s="8"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="29"/>
       <c r="C30" s="8" t="s">
         <v>59</v>
       </c>
@@ -1647,22 +1680,22 @@
       <c r="E30" s="10">
         <v>43727</v>
       </c>
-      <c r="F30" s="25"/>
+      <c r="F30" s="30"/>
       <c r="G30" s="10">
         <v>43727</v>
       </c>
       <c r="H30" s="10">
         <v>43727</v>
       </c>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
       <c r="K30" s="8"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="24">
+      <c r="A31" s="29">
         <v>6</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="29" t="s">
         <v>63</v>
       </c>
       <c r="C31" s="8" t="s">
@@ -1674,7 +1707,7 @@
       <c r="E31" s="10">
         <v>43756</v>
       </c>
-      <c r="F31" s="25">
+      <c r="F31" s="30">
         <v>43760</v>
       </c>
       <c r="G31" s="10">
@@ -1683,7 +1716,7 @@
       <c r="H31" s="10">
         <v>43760</v>
       </c>
-      <c r="I31" s="24">
+      <c r="I31" s="29">
         <v>100</v>
       </c>
       <c r="J31" s="8" t="s">
@@ -1692,8 +1725,8 @@
       <c r="K31" s="8"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
-      <c r="B32" s="24"/>
+      <c r="A32" s="29"/>
+      <c r="B32" s="29"/>
       <c r="C32" s="8" t="s">
         <v>64</v>
       </c>
@@ -1703,22 +1736,22 @@
       <c r="E32" s="10">
         <v>43758</v>
       </c>
-      <c r="F32" s="25"/>
+      <c r="F32" s="30"/>
       <c r="G32" s="10">
         <v>43760</v>
       </c>
       <c r="H32" s="10">
         <v>43760</v>
       </c>
-      <c r="I32" s="24"/>
-      <c r="J32" s="24" t="s">
+      <c r="I32" s="29"/>
+      <c r="J32" s="29" t="s">
         <v>22</v>
       </c>
       <c r="K32" s="8"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
-      <c r="B33" s="24"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="29"/>
       <c r="C33" s="8" t="s">
         <v>65</v>
       </c>
@@ -1728,15 +1761,15 @@
       <c r="E33" s="10">
         <v>43760</v>
       </c>
-      <c r="F33" s="25"/>
+      <c r="F33" s="30"/>
       <c r="G33" s="10">
         <v>43761</v>
       </c>
       <c r="H33" s="10">
         <v>43761</v>
       </c>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
       <c r="K33" s="8"/>
     </row>
   </sheetData>
@@ -1751,12 +1784,25 @@
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="E12:E17"/>
+    <mergeCell ref="E22:E28"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="F9:F11"/>
     <mergeCell ref="I9:I11"/>
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="H5:H6"/>
+    <mergeCell ref="A12:A21"/>
+    <mergeCell ref="A22:A30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="J22:J30"/>
+    <mergeCell ref="F31:F33"/>
     <mergeCell ref="B12:B21"/>
     <mergeCell ref="B22:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -1766,19 +1812,6 @@
     <mergeCell ref="F22:F30"/>
     <mergeCell ref="I12:I21"/>
     <mergeCell ref="I22:I30"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="E12:E17"/>
-    <mergeCell ref="E22:E28"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="J22:J30"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A21"/>
-    <mergeCell ref="A22:A30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1787,73 +1820,75 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.28515625" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" customWidth="1"/>
-    <col min="9" max="9" width="26.42578125" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" customWidth="1"/>
+    <col min="4" max="5" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="34"/>
       <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="36"/>
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="J1" s="1"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
+      <c r="B2" s="35"/>
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="36"/>
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" s="1"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
@@ -1866,30 +1901,33 @@
       <c r="D4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="G4" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="H4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="J4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="K4" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="40">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="48">
         <v>1</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="48" t="s">
         <v>77</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -1898,40 +1936,42 @@
       <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="28"/>
+      <c r="F5" s="46">
         <v>43766</v>
       </c>
-      <c r="F5" s="38">
+      <c r="G5" s="46">
         <v>43766</v>
       </c>
-      <c r="G5" s="38">
+      <c r="H5" s="46">
         <v>43766</v>
       </c>
-      <c r="H5" s="39">
+      <c r="I5" s="47">
         <v>100</v>
       </c>
-      <c r="I5" s="40" t="s">
+      <c r="J5" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="48"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="21" t="s">
         <v>79</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E6" s="28"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>2</v>
       </c>
@@ -1944,28 +1984,29 @@
       <c r="D7" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="23">
-        <v>43717</v>
-      </c>
+      <c r="E7" s="28"/>
       <c r="F7" s="23">
         <v>43717</v>
       </c>
       <c r="G7" s="23">
+        <v>43717</v>
+      </c>
+      <c r="H7" s="23">
         <v>43716</v>
       </c>
-      <c r="H7" s="6">
+      <c r="I7" s="6">
         <v>100</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="J7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="29">
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="37">
         <v>3</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="37" t="s">
         <v>80</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -1974,154 +2015,199 @@
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="27">
+        <v>43758</v>
+      </c>
+      <c r="F8" s="43">
         <v>43785</v>
-      </c>
-      <c r="F8" s="23">
-        <v>43758</v>
       </c>
       <c r="G8" s="23">
         <v>43758</v>
       </c>
-      <c r="H8" s="41">
+      <c r="H8" s="23">
+        <v>43758</v>
+      </c>
+      <c r="I8" s="49">
         <v>100</v>
       </c>
-      <c r="I8" s="40" t="s">
+      <c r="J8" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="32" t="s">
+      <c r="K8" s="40" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="5" t="s">
         <v>84</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="23">
-        <v>43758</v>
-      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="44"/>
       <c r="G9" s="23">
         <v>43758</v>
       </c>
-      <c r="H9" s="42"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="33"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
+      <c r="H9" s="23">
+        <v>43758</v>
+      </c>
+      <c r="I9" s="50"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="41"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="5" t="s">
         <v>85</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="23">
-        <v>43785</v>
-      </c>
+      <c r="E10" s="25"/>
+      <c r="F10" s="44"/>
       <c r="G10" s="23">
         <v>43785</v>
       </c>
-      <c r="H10" s="43"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="33"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
+      <c r="H10" s="23">
+        <v>43785</v>
+      </c>
+      <c r="I10" s="51"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="41"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="38"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="5" t="s">
         <v>87</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="23">
-        <v>43785</v>
-      </c>
+      <c r="E11" s="25"/>
+      <c r="F11" s="44"/>
       <c r="G11" s="23">
         <v>43785</v>
       </c>
-      <c r="H11" s="5"/>
+      <c r="H11" s="23">
+        <v>43785</v>
+      </c>
       <c r="I11" s="5"/>
-      <c r="J11" s="33"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="41"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="39"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="5" t="s">
         <v>88</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E12" s="37"/>
-      <c r="F12" s="23">
-        <v>43785</v>
-      </c>
+      <c r="E12" s="26"/>
+      <c r="F12" s="45"/>
       <c r="G12" s="23">
         <v>43785</v>
       </c>
-      <c r="H12" s="5"/>
+      <c r="H12" s="23">
+        <v>43785</v>
+      </c>
       <c r="I12" s="5"/>
-      <c r="J12" s="34"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="42"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>4</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="52">
+        <v>43789</v>
+      </c>
+      <c r="F13" s="52">
+        <v>43802</v>
+      </c>
+      <c r="G13" s="52">
+        <v>43802</v>
+      </c>
+      <c r="H13" s="52">
+        <v>43794</v>
+      </c>
       <c r="I13" s="13"/>
-      <c r="J13" s="14"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13" s="13"/>
+      <c r="K13" s="14"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
+      <c r="C14" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
+      <c r="H14" s="52">
+        <v>43795</v>
+      </c>
       <c r="I14" s="16"/>
-      <c r="J14" s="17"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J14" s="16"/>
+      <c r="K14" s="17"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
+      <c r="C15" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
+      <c r="H15" s="52">
+        <v>43796</v>
+      </c>
       <c r="I15" s="16"/>
-      <c r="J15" s="17"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J15" s="16"/>
+      <c r="K15" s="17"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+      <c r="C16" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>96</v>
+      </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
+      <c r="H16" s="52">
+        <v>43797</v>
+      </c>
       <c r="I16" s="16"/>
-      <c r="J16" s="17"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" s="16"/>
+      <c r="K16" s="17"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -2131,9 +2217,10 @@
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
       <c r="I17" s="16"/>
-      <c r="J17" s="17"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J17" s="16"/>
+      <c r="K17" s="17"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -2143,9 +2230,10 @@
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
       <c r="I18" s="16"/>
-      <c r="J18" s="17"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J18" s="16"/>
+      <c r="K18" s="17"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -2155,9 +2243,10 @@
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
       <c r="I19" s="16"/>
-      <c r="J19" s="17"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J19" s="16"/>
+      <c r="K19" s="17"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -2167,9 +2256,10 @@
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>
-      <c r="J20" s="17"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J20" s="16"/>
+      <c r="K20" s="17"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -2179,9 +2269,10 @@
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
       <c r="I21" s="16"/>
-      <c r="J21" s="17"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J21" s="16"/>
+      <c r="K21" s="17"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -2191,9 +2282,10 @@
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
-      <c r="J22" s="17"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J22" s="16"/>
+      <c r="K22" s="17"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -2203,9 +2295,10 @@
       <c r="G23" s="16"/>
       <c r="H23" s="16"/>
       <c r="I23" s="16"/>
-      <c r="J23" s="17"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J23" s="16"/>
+      <c r="K23" s="17"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
@@ -2215,9 +2308,10 @@
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
-      <c r="J24" s="17"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J24" s="16"/>
+      <c r="K24" s="17"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -2227,9 +2321,10 @@
       <c r="G25" s="16"/>
       <c r="H25" s="16"/>
       <c r="I25" s="16"/>
-      <c r="J25" s="17"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J25" s="16"/>
+      <c r="K25" s="17"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -2239,9 +2334,10 @@
       <c r="G26" s="16"/>
       <c r="H26" s="16"/>
       <c r="I26" s="16"/>
-      <c r="J26" s="17"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J26" s="16"/>
+      <c r="K26" s="17"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -2251,9 +2347,10 @@
       <c r="G27" s="16"/>
       <c r="H27" s="16"/>
       <c r="I27" s="16"/>
-      <c r="J27" s="17"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J27" s="16"/>
+      <c r="K27" s="17"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -2263,9 +2360,10 @@
       <c r="G28" s="16"/>
       <c r="H28" s="16"/>
       <c r="I28" s="16"/>
-      <c r="J28" s="17"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J28" s="16"/>
+      <c r="K28" s="17"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
@@ -2275,9 +2373,10 @@
       <c r="G29" s="16"/>
       <c r="H29" s="16"/>
       <c r="I29" s="16"/>
-      <c r="J29" s="17"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J29" s="16"/>
+      <c r="K29" s="17"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
@@ -2287,9 +2386,10 @@
       <c r="G30" s="16"/>
       <c r="H30" s="16"/>
       <c r="I30" s="16"/>
-      <c r="J30" s="17"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J30" s="16"/>
+      <c r="K30" s="17"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -2299,9 +2399,10 @@
       <c r="G31" s="16"/>
       <c r="H31" s="16"/>
       <c r="I31" s="16"/>
-      <c r="J31" s="17"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J31" s="16"/>
+      <c r="K31" s="17"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -2311,9 +2412,10 @@
       <c r="G32" s="16"/>
       <c r="H32" s="16"/>
       <c r="I32" s="16"/>
-      <c r="J32" s="17"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J32" s="16"/>
+      <c r="K32" s="17"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
@@ -2323,9 +2425,10 @@
       <c r="G33" s="16"/>
       <c r="H33" s="16"/>
       <c r="I33" s="16"/>
-      <c r="J33" s="17"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J33" s="16"/>
+      <c r="K33" s="17"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
@@ -2335,27 +2438,28 @@
       <c r="G34" s="19"/>
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
-      <c r="J34" s="20"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="17">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="F2:G2"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
     <mergeCell ref="B8:B12"/>
     <mergeCell ref="A8:A12"/>
-    <mergeCell ref="J8:J12"/>
-    <mergeCell ref="E8:E12"/>
-    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="K8:K12"/>
+    <mergeCell ref="F8:F12"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="I5:I6"/>
-    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="J5:J6"/>
     <mergeCell ref="I8:I10"/>
+    <mergeCell ref="J8:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>